<commit_message>
Started working on Songmap and Songmap controller.
Added initial attributes to Songmap and started working on songmap serialization/deserialization from xml.
</commit_message>
<xml_diff>
--- a/work_hours.xlsx
+++ b/work_hours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Documents\OAMK\2019\Projects\AudioSamurai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B0B04B-A3A5-42E5-87C9-081795C02195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC75C79-8F0A-4942-9381-7295A2DD3EBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lokakuu" sheetId="1" r:id="rId1"/>
@@ -77,8 +77,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="d/m/yy;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -488,31 +488,31 @@
     <xf numFmtId="2" fontId="3" fillId="6" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="6" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="6" borderId="16" xfId="5" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="5" borderId="14" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="5" borderId="15" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="5" borderId="17" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="14" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="15" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="17" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1"/>
-    <xf numFmtId="167" fontId="3" fillId="6" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="3" fillId="6" borderId="16" xfId="5" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="16" xfId="5" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="21" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20 % - Aksentti1" xfId="1" builtinId="30"/>
@@ -800,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,19 +848,19 @@
         <v>43766</v>
       </c>
       <c r="C3" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3" s="10">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -868,7 +868,7 @@
         <v>43767</v>
       </c>
       <c r="C4" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D4" s="9">
         <v>0</v>
@@ -929,27 +929,27 @@
       </c>
       <c r="C7" s="5">
         <f>SUM(C3:C6)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D7" s="5">
         <f>SUM(D3:D6)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7" s="5">
         <f>SUM(E3:E6)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="5">
         <f>SUM(F3:F6)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7" s="12">
         <f>SUM(G3:G6)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7" s="13">
         <f>SUM(C7:G7)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1647,7 +1647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CEE12E-FA02-47A2-8FAB-9C1BBCEE2490}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -2390,23 +2390,23 @@
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="30">
         <f>SUM(Lokakuu!C7,Marraskuu!C33,Joulukuu!C34)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C5" s="31">
         <f>SUM(Lokakuu!D7,Marraskuu!D33,Joulukuu!D34)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5" s="31">
         <f>SUM(Lokakuu!E7,Marraskuu!E33,Joulukuu!E34)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5" s="31">
         <f>SUM(Lokakuu!F7,Marraskuu!F33,Joulukuu!F34)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="32">
         <f>SUM(Lokakuu!G7,Marraskuu!G33,Joulukuu!G34)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished intial version of XML serialization/deserialization
Songmaps can now be serialized automatically to the correct folder in %localappdata%/AudioSamurai/Songs based on the map information.
</commit_message>
<xml_diff>
--- a/work_hours.xlsx
+++ b/work_hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Documents\OAMK\2019\Projects\AudioSamurai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC75C79-8F0A-4942-9381-7295A2DD3EBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFBA276-CBA8-4EAE-9548-2F9C5624C979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -801,7 +801,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,7 +888,7 @@
         <v>43768</v>
       </c>
       <c r="C5" s="8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D5" s="9">
         <v>0</v>
@@ -908,7 +908,7 @@
         <v>43769</v>
       </c>
       <c r="C6" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" s="9">
         <v>0</v>
@@ -929,7 +929,7 @@
       </c>
       <c r="C7" s="5">
         <f>SUM(C3:C6)</f>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D7" s="5">
         <f>SUM(D3:D6)</f>
@@ -949,7 +949,7 @@
       </c>
       <c r="H7" s="13">
         <f>SUM(C7:G7)</f>
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2390,7 +2390,7 @@
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="30">
         <f>SUM(Lokakuu!C7,Marraskuu!C33,Joulukuu!C34)</f>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C5" s="31">
         <f>SUM(Lokakuu!D7,Marraskuu!D33,Joulukuu!D34)</f>

</xml_diff>